<commit_message>
useful document from 310
</commit_message>
<xml_diff>
--- a/Tests/Mixer_with_BPF/Data.xlsx
+++ b/Tests/Mixer_with_BPF/Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://rosehulman-my.sharepoint.com/personal/gardneml_rose-hulman_edu/Documents/Desktop/Senior Design/Tests/Mixer_with_BPF/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="83" documentId="11_F25DC773A252ABDACC1048E721DB5AF65BDE58F2" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3C63291B-CA10-4E3B-BE0F-3B97A396BE8C}"/>
+  <xr:revisionPtr revIDLastSave="92" documentId="11_F25DC773A252ABDACC1048E721DB5AF65BDE58F2" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FBED4C79-75B1-43EC-94EF-81171947655D}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3108" yWindow="3252" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -386,7 +386,7 @@
   <dimension ref="A1:J14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+      <selection activeCell="H2" activeCellId="1" sqref="B2:B14 H2:H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -552,7 +552,7 @@
         <v>-69</v>
       </c>
       <c r="I5">
-        <f t="shared" si="2"/>
+        <f>H5-G5</f>
         <v>-14</v>
       </c>
     </row>
@@ -654,7 +654,7 @@
         <v>-75</v>
       </c>
       <c r="I8">
-        <f t="shared" si="2"/>
+        <f>H8-G8</f>
         <v>-23</v>
       </c>
     </row>
@@ -686,7 +686,7 @@
         <v>-69</v>
       </c>
       <c r="I9">
-        <f t="shared" si="2"/>
+        <f>H9-G9</f>
         <v>-14</v>
       </c>
       <c r="J9" t="s">

</xml_diff>